<commit_message>
reaction in STN manager introduced
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_ja/lab_app_ja_knowledge.xlsx
+++ b/sample_apps/lab_app_ja/lab_app_ja_knowledge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-0.3.1\sample_apps\lab_app_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1E5DC6-8CCF-4110-A154-76B54CCE87C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A10E19-D252-4375-8271-6B204C3C8FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="145">
   <si>
     <t>system utterance</t>
     <phoneticPr fontId="1"/>
@@ -241,19 +241,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>そうなんですね。好きじゃないのに何で食べるのですか？</t>
-    <rPh sb="8" eb="9">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>ナン</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>タ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>安いから</t>
     <rPh sb="0" eb="1">
       <t>ヤス</t>
@@ -912,6 +899,33 @@
   </si>
   <si>
     <t>_set(&amp;confirmation_request, "すみません。ラーメンってよく食べますか？")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>好きじゃないのに何で食べるのですか？</t>
+    <rPh sb="0" eb="1">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ナン</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>タ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_set(&amp;_reaction, "そうなんですか。")</t>
+  </si>
+  <si>
+    <t>_set(&amp;_reaction, "そうなんですか。")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_set(&amp;_reaction, "そうなんですね。")</t>
+  </si>
+  <si>
+    <t>_set(&amp;_reaction, "そうなんですね。")</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1388,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1410,7 +1424,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
@@ -1433,15 +1447,15 @@
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="G2" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>22</v>
@@ -1449,13 +1463,13 @@
     </row>
     <row r="3" spans="1:8" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>14</v>
@@ -1470,7 +1484,7 @@
     </row>
     <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>22</v>
@@ -1489,7 +1503,7 @@
     </row>
     <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>22</v>
@@ -1508,7 +1522,7 @@
     </row>
     <row r="6" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>22</v>
@@ -1516,25 +1530,25 @@
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="G6" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" s="7"/>
       <c r="F7" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="6" t="s">
@@ -1543,15 +1557,15 @@
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="F8" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="6" t="s">
@@ -1560,7 +1574,7 @@
     </row>
     <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>2</v>
@@ -1574,14 +1588,16 @@
       <c r="E9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>144</v>
+      </c>
       <c r="H9" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>2</v>
@@ -1593,14 +1609,16 @@
       <c r="E10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="H10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>2</v>
@@ -1612,14 +1630,16 @@
       <c r="E11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="13" t="s">
+        <v>142</v>
+      </c>
       <c r="H11" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>2</v>
@@ -1631,30 +1651,34 @@
       <c r="E12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="H12" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" s="13"/>
+        <v>98</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="H13" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>3</v>
@@ -1672,7 +1696,7 @@
     </row>
     <row r="15" spans="1:8" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>26</v>
@@ -1687,10 +1711,10 @@
         <v>31</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>21</v>
@@ -1698,7 +1722,7 @@
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>26</v>
@@ -1711,10 +1735,10 @@
         <v>31</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>31</v>
@@ -1722,7 +1746,7 @@
     </row>
     <row r="17" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>26</v>
@@ -1733,25 +1757,25 @@
         <v>31</v>
       </c>
       <c r="F17" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>102</v>
-      </c>
       <c r="H17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A18" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="10" t="s">
@@ -1760,16 +1784,16 @@
     </row>
     <row r="19" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A19" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="G19" s="11"/>
       <c r="H19" s="10" t="s">
@@ -1778,31 +1802,31 @@
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D20" s="7"/>
       <c r="G20" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A21" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="9"/>
       <c r="G21" s="9"/>
@@ -1812,33 +1836,33 @@
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="E22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1849,104 +1873,104 @@
     </row>
     <row r="24" spans="1:8" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A24" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>110</v>
       </c>
       <c r="D24" s="13"/>
       <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="D25" s="9"/>
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="11"/>
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A28" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="D28" s="11"/>
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="G30" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.4">
@@ -1986,475 +2010,475 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
@@ -2490,32 +2514,32 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
         <v>112</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>113</v>
-      </c>
-      <c r="C3" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2545,24 +2569,24 @@
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2576,10 +2600,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -2617,83 +2641,83 @@
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
         <v>93</v>
-      </c>
-      <c r="D6" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
builtin spacy ner block added
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_ja/lab_app_ja_knowledge.xlsx
+++ b/sample_apps/lab_app_ja/lab_app_ja_knowledge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-0.3.1\sample_apps\lab_app_ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-pub-dev\sample_apps\lab_app_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A10E19-D252-4375-8271-6B204C3C8FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6FD5FF-C553-48F0-ACF5-24B532B35247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15870" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="152">
   <si>
     <t>system utterance</t>
     <phoneticPr fontId="1"/>
@@ -894,10 +894,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{greeting}。今日はラーメンについて教えて下さい。ラーメンはよく食べますか？</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>_set(&amp;confirmation_request, "すみません。ラーメンってよく食べますか？")</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -926,6 +922,68 @@
   </si>
   <si>
     <t>_set(&amp;_reaction, "そうなんですね。")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{greeting}。私はチャットボットです。よろしければお名前を教えて頂けますか？</t>
+    <rPh sb="11" eb="12">
+      <t>ワタシ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>オシ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>イタダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>田中です。</t>
+    <rPh sb="0" eb="2">
+      <t>タナカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_ne(#NE_Person, "")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_set(&amp;user_name, #NE_Person)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名前を言った</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名前を取れなかった</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ありがとうございます。{user_name}さん、今日はラーメンについて教えて下さい。ラーメンはよく食べますか？</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>すみません、ちょっと理解できませんでした。今日はラーメンについて教えて下さい。ラーメンはよく食べますか？</t>
+    <rPh sb="10" eb="12">
+      <t>リカイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -958,7 +1016,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1007,6 +1065,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1037,7 +1107,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1084,6 +1154,24 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1400,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1461,520 +1549,624 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+      <c r="A5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="18" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A8" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="G8" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="H8" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+      <c r="A9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="10" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11" t="s">
+    <row r="10" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E10" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="10" t="s">
+      <c r="G10" s="21"/>
+      <c r="H10" s="20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
+    <row r="11" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="10" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="G6" s="11" t="s">
+    <row r="12" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A12" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="G12" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="F13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="F14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+      <c r="A21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="F7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="F8" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="D25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A30" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A34" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="11"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.4">
-      <c r="A15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A18" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="G20" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A21" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A24" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" s="10" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A28" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="8" t="s">
+      <c r="G35" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="H29" s="8" t="s">
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="G36" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="G30" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.4">
-      <c r="C35" s="14"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C41" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
OPENAI_API_KEY, new builtin functions added
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_ja/lab_app_ja_knowledge.xlsx
+++ b/sample_apps/lab_app_ja/lab_app_ja_knowledge.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-v0.7\sample_apps\lab_app_ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2ECF98-800C-4C51-8797-DA6E611C1D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38827274-E128-4060-A069-CBACAAB5D648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="19185" windowHeight="10335" activeTab="2" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="33510" yWindow="1395" windowWidth="21600" windowHeight="11505" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -665,22 +665,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{greeting}。私はチャットボットです。よろしければお名前を教えて頂けますか？</t>
-    <rPh sb="11" eb="12">
-      <t>ワタシ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>ナマエ</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>オシ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>イタダ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>田中です。</t>
     <rPh sb="0" eb="2">
       <t>タナカ</t>
@@ -984,6 +968,22 @@
     </rPh>
     <rPh sb="15" eb="17">
       <t>ミソ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{greeting}。私は{get_name()}です。よろしければお名前を教えて頂けますか？</t>
+    <rPh sb="11" eb="12">
+      <t>ワタシ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>オシ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>イタダ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1190,9 +1190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1230,7 +1230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1336,7 +1336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1478,7 +1478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1488,24 +1488,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" style="13"/>
+    <col min="1" max="1" width="8.625" style="13"/>
     <col min="2" max="2" width="25.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.58203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.875" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.25" style="13" customWidth="1"/>
     <col min="6" max="6" width="33.5" style="13" customWidth="1"/>
     <col min="7" max="7" width="39" style="14" customWidth="1"/>
-    <col min="8" max="8" width="37.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.58203125" style="13"/>
+    <col min="8" max="8" width="37.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>35</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="15" customFormat="1" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" s="15" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>35</v>
       </c>
@@ -1555,22 +1555,22 @@
         <v>21</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>35</v>
       </c>
@@ -1581,28 +1581,28 @@
       <c r="D4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="17" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+      <c r="A5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>108</v>
       </c>
       <c r="D5" s="18"/>
       <c r="G5" s="18"/>
     </row>
-    <row r="6" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18" t="s">
@@ -1616,12 +1616,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18" t="s">
@@ -1635,12 +1635,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="17" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A8" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
@@ -1648,18 +1648,18 @@
         <v>96</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="19" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.4">
       <c r="A9" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>13</v>
@@ -1672,12 +1672,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20" t="s">
@@ -1691,12 +1691,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20" t="s">
@@ -1710,12 +1710,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" s="19" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A12" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -1726,7 +1726,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="11" t="s">
         <v>35</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="11" t="s">
         <v>35</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
         <v>35</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
         <v>35</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11" t="s">
         <v>35</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>35</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="9" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
@@ -1901,16 +1901,16 @@
         <v>30</v>
       </c>
       <c r="F21" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="9" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" s="9" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A22" s="9" t="s">
         <v>35</v>
       </c>
@@ -1925,16 +1925,16 @@
         <v>30</v>
       </c>
       <c r="F22" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
         <v>35</v>
       </c>
@@ -1947,16 +1947,16 @@
         <v>30</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="9" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A24" s="9" t="s">
         <v>35</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="9" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A25" s="9" t="s">
         <v>35</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>35</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A27" s="7" t="s">
         <v>35</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>35</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>35</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" s="11" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A30" s="11" t="s">
         <v>35</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="D30" s="12"/>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
@@ -2087,7 +2087,7 @@
       <c r="D31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="9" t="s">
         <v>35</v>
       </c>
@@ -2100,7 +2100,7 @@
       <c r="D32" s="10"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:8" s="5" customFormat="1" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="D33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:8" s="9" customFormat="1" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" s="9" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A34" s="9" t="s">
         <v>35</v>
       </c>
@@ -2121,12 +2121,12 @@
         <v>82</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D34" s="10"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="7" t="s">
         <v>35</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C41" s="13"/>
     </row>
   </sheetData>
@@ -2181,14 +2181,14 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="31.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2199,10 +2199,10 @@
         <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2408,13 +2408,13 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2422,13 +2422,13 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2436,80 +2436,80 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
         <v>118</v>
       </c>
-      <c r="D22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" t="s">
         <v>119</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" t="s">
         <v>120</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C25" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" t="s">
-        <v>115</v>
-      </c>
-      <c r="D26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>128</v>
-      </c>
-      <c r="D27" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2523,17 +2523,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E27BD90-5E4C-4A7C-B9E8-ABC211947ECB}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2547,12 +2547,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -2561,12 +2561,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
         <v>59</v>
@@ -2575,12 +2575,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
         <v>60</v>
@@ -2589,12 +2589,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
         <v>65</v>
@@ -2603,12 +2603,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
         <v>66</v>
@@ -2617,37 +2617,37 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
examples of builtin chatgpt functions
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_ja/lab_app_ja_knowledge.xlsx
+++ b/sample_apps/lab_app_ja/lab_app_ja_knowledge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABB7C51-64E4-43F7-B596-A0A4CFF68B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD80C601-D008-409D-90EE-242CEF42CC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="144">
   <si>
     <t>system utterance</t>
     <phoneticPr fontId="1"/>
@@ -266,10 +266,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>わかりました。今日はお時間ありがとうございました。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>近所の街中華のラーメンが好きなんだよね</t>
     <rPh sb="0" eb="2">
       <t>キンジョ</t>
@@ -984,6 +980,34 @@
     </rPh>
     <rPh sb="48" eb="49">
       <t>イタダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#final_apology</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>すみません。よくわかりませんでした。とりあえず今日はここまでにさせてください。ありがとうございました。</t>
+    <rPh sb="23" eb="25">
+      <t>キョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_check_with_chatgpt("ユーザが理由を言ったかどうか判断してください。")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>わかりました。{_generate_with_chatgpt("それまでの会話につづけて、対話を終わらせる発話を50文字以内で生成してください。")}今日はお時間ありがとうございました。</t>
+    <rPh sb="45" eb="47">
+      <t>タイワ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>イナイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1486,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1499,7 +1523,7 @@
     <col min="3" max="3" width="29.625" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.875" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.25" style="13" customWidth="1"/>
-    <col min="6" max="6" width="33.5" style="13" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="14" customWidth="1"/>
     <col min="7" max="7" width="39" style="14" customWidth="1"/>
     <col min="8" max="8" width="37.875" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.625" style="13"/>
@@ -1510,7 +1534,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -1521,7 +1545,7 @@
       <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -1536,12 +1560,13 @@
         <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>21</v>
@@ -1555,19 +1580,19 @@
         <v>21</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.4">
@@ -1579,9 +1604,10 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="17" customFormat="1" ht="75" x14ac:dyDescent="0.4">
@@ -1589,12 +1615,13 @@
         <v>35</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="18"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.4">
@@ -1602,7 +1629,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18" t="s">
@@ -1611,6 +1638,7 @@
       <c r="E6" s="17" t="s">
         <v>3</v>
       </c>
+      <c r="F6" s="18"/>
       <c r="G6" s="18"/>
       <c r="H6" s="17" t="s">
         <v>3</v>
@@ -1621,7 +1649,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18" t="s">
@@ -1630,6 +1658,7 @@
       <c r="E7" s="17" t="s">
         <v>19</v>
       </c>
+      <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="17" t="s">
         <v>2</v>
@@ -1640,15 +1669,16 @@
         <v>35</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.4">
@@ -1656,10 +1686,10 @@
         <v>35</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>13</v>
@@ -1667,6 +1697,7 @@
       <c r="E9" s="19" t="s">
         <v>2</v>
       </c>
+      <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="19" t="s">
         <v>2</v>
@@ -1677,7 +1708,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20" t="s">
@@ -1686,6 +1717,7 @@
       <c r="E10" s="19" t="s">
         <v>3</v>
       </c>
+      <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="19" t="s">
         <v>3</v>
@@ -1696,7 +1728,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20" t="s">
@@ -1705,6 +1737,7 @@
       <c r="E11" s="19" t="s">
         <v>19</v>
       </c>
+      <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="19" t="s">
         <v>2</v>
@@ -1715,15 +1748,16 @@
         <v>35</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -1731,14 +1765,14 @@
         <v>35</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="F13" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="F13" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="5" t="s">
@@ -1750,12 +1784,12 @@
         <v>35</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="F14" s="5" t="s">
-        <v>89</v>
+      <c r="F14" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="5" t="s">
@@ -1778,8 +1812,9 @@
       <c r="E15" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="F15" s="12"/>
       <c r="G15" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>25</v>
@@ -1799,8 +1834,9 @@
       <c r="E16" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="F16" s="12"/>
       <c r="G16" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>25</v>
@@ -1820,8 +1856,9 @@
       <c r="E17" s="11" t="s">
         <v>26</v>
       </c>
+      <c r="F17" s="12"/>
       <c r="G17" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>27</v>
@@ -1841,8 +1878,9 @@
       <c r="E18" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>27</v>
@@ -1857,10 +1895,11 @@
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
-        <v>71</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F19" s="12"/>
       <c r="G19" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>25</v>
@@ -1879,6 +1918,7 @@
       <c r="D20" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="7" t="s">
         <v>22</v>
@@ -1900,11 +1940,11 @@
       <c r="E21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>134</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>20</v>
@@ -1924,11 +1964,11 @@
       <c r="E22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>136</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>30</v>
@@ -1946,14 +1986,14 @@
       <c r="E23" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>137</v>
+      <c r="F23" s="10" t="s">
+        <v>136</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
@@ -1965,14 +2005,15 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>37</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" s="9" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A25" s="9" t="s">
         <v>35</v>
       </c>
@@ -1980,191 +2021,231 @@
         <v>27</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="F25" s="10" t="s">
+        <v>142</v>
+      </c>
       <c r="G25" s="10"/>
       <c r="H25" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="5" t="s">
+    <row r="27" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="G26" s="6" t="s">
+      <c r="C27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H26" s="5" t="s">
+    </row>
+    <row r="28" spans="1:8" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="11" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A31" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="7" t="s">
+      <c r="D32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" s="9" customFormat="1" ht="112.5" x14ac:dyDescent="0.4">
+      <c r="A33" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A28" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="6" t="s">
+      <c r="C33" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+      <c r="A34" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" s="9" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A36" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="H28" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="11" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A30" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="G30" s="12"/>
-    </row>
-    <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="10"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="1:8" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:8" s="9" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A34" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="7" t="s">
+      <c r="C36" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="D37" s="8"/>
+      <c r="E37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="8" t="s">
+    </row>
+    <row r="38" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H35" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="G36" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C41" s="13"/>
+      <c r="H38" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2199,7 +2280,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -2210,7 +2291,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -2221,7 +2302,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
@@ -2232,7 +2313,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
@@ -2243,7 +2324,7 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -2254,7 +2335,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -2265,7 +2346,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
@@ -2276,7 +2357,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -2287,7 +2368,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
@@ -2298,7 +2379,7 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -2309,7 +2390,7 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
@@ -2320,7 +2401,7 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
@@ -2331,7 +2412,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
@@ -2342,7 +2423,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
@@ -2353,7 +2434,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
@@ -2364,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
@@ -2375,7 +2456,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
@@ -2386,7 +2467,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
@@ -2397,7 +2478,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
@@ -2408,10 +2489,10 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
@@ -2422,10 +2503,10 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
@@ -2436,10 +2517,10 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
@@ -2447,13 +2528,13 @@
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
@@ -2461,13 +2542,13 @@
         <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
@@ -2475,13 +2556,13 @@
         <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
@@ -2489,13 +2570,13 @@
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
-        <v>114</v>
-      </c>
       <c r="D26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
@@ -2503,13 +2584,13 @@
         <v>35</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" t="s">
         <v>127</v>
-      </c>
-      <c r="D27" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2538,27 +2619,27 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -2566,13 +2647,13 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
@@ -2580,13 +2661,13 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
@@ -2594,13 +2675,13 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -2608,13 +2689,13 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
         <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -2622,10 +2703,10 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
@@ -2633,10 +2714,10 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -2644,10 +2725,10 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>